<commit_message>
Test case Id Update
</commit_message>
<xml_diff>
--- a/E-boighar_bugReport.xlsx
+++ b/E-boighar_bugReport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA B-16\Eboighar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA B-16\all_project_git\Eboighar testing\E-boighar-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -116,9 +116,6 @@
     <t>User should get warning "please user strong password" and should not able to use weak password.</t>
   </si>
   <si>
-    <t>User not got any warning message .</t>
-  </si>
-  <si>
     <t>Validate Password field into minimum leanght.</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>1. User not got any warning message. And user able to use less than 8 character password.</t>
+  </si>
+  <si>
+    <t>User not got any warning message.</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
@@ -723,13 +723,13 @@
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
@@ -741,19 +741,19 @@
     </row>
     <row r="5" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>8</v>

</xml_diff>